<commit_message>
xlxs for freelancer, k=0.1, k=2
</commit_message>
<xml_diff>
--- a/results/real_data_freelancer_0.1_opt_constrained/k=0.1/CSG/dataset_05/results_excel_26-9-22_freelancer_constrained_1_.xlsx
+++ b/results/real_data_freelancer_0.1_opt_constrained/k=0.1/CSG/dataset_05/results_excel_26-9-22_freelancer_constrained_1_.xlsx
@@ -1,20 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Konstantina\Desktop\HDrop20-Master-Thesis-Experiments\results\real_data_freelancer_0.1_opt_constrained\k=0.1\CSG\dataset_05\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA06383D-542D-4D58-B6BB-6C303B6E2D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>dataset</t>
   </si>
@@ -122,13 +141,25 @@
   </si>
   <si>
     <t>Official_Experiment_CSG_dataset_05_instance_10_9_exec</t>
+  </si>
+  <si>
+    <t>Average of SW(S*)/SW(OPT)</t>
+  </si>
+  <si>
+    <t>Average of SC(S*)/SC(OPT)</t>
+  </si>
+  <si>
+    <t>Worst of SW(S*)/SW(OPT)</t>
+  </si>
+  <si>
+    <t>Worst of SC(S*)/SC(OPT)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +173,24 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -180,22 +229,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -237,7 +298,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -269,9 +330,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -303,6 +382,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -478,14 +575,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -562,7 +661,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -612,10 +711,10 @@
         <v>20</v>
       </c>
       <c r="Q2">
-        <v>2.48073127837752</v>
+        <v>2.4807312783775202</v>
       </c>
       <c r="R2">
-        <v>169.3853744324496</v>
+        <v>169.38537443244959</v>
       </c>
       <c r="S2">
         <v>11.95</v>
@@ -624,10 +723,10 @@
         <v>11.95</v>
       </c>
       <c r="U2">
-        <v>2.48073127837752</v>
+        <v>2.4807312783775202</v>
       </c>
       <c r="V2">
-        <v>169.3853744324496</v>
+        <v>169.38537443244959</v>
       </c>
       <c r="W2">
         <v>512</v>
@@ -642,7 +741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -695,7 +794,7 @@
         <v>2.763169500323289</v>
       </c>
       <c r="R3">
-        <v>241.7366099935342</v>
+        <v>241.73660999353419</v>
       </c>
       <c r="S3">
         <v>15.85</v>
@@ -707,7 +806,7 @@
         <v>2.763169500323289</v>
       </c>
       <c r="V3">
-        <v>241.7366099935342</v>
+        <v>241.73660999353419</v>
       </c>
       <c r="W3">
         <v>829</v>
@@ -722,7 +821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -772,10 +871,10 @@
         <v>5</v>
       </c>
       <c r="Q4">
-        <v>2.785011242238338</v>
+        <v>2.7850112422383382</v>
       </c>
       <c r="R4">
-        <v>62.07494378880831</v>
+        <v>62.074943788808312</v>
       </c>
       <c r="S4">
         <v>16.2</v>
@@ -784,10 +883,10 @@
         <v>16.2</v>
       </c>
       <c r="U4">
-        <v>2.785011242238338</v>
+        <v>2.7850112422383382</v>
       </c>
       <c r="V4">
-        <v>62.07494378880831</v>
+        <v>62.074943788808312</v>
       </c>
       <c r="W4">
         <v>516</v>
@@ -802,7 +901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -852,10 +951,10 @@
         <v>13</v>
       </c>
       <c r="Q5">
-        <v>2.332890442489375</v>
+        <v>2.3328904424893748</v>
       </c>
       <c r="R5">
-        <v>90.67242424763813</v>
+        <v>90.672424247638133</v>
       </c>
       <c r="S5">
         <v>10.30769230769231</v>
@@ -864,10 +963,10 @@
         <v>10.30769230769231</v>
       </c>
       <c r="U5">
-        <v>2.332890442489375</v>
+        <v>2.3328904424893748</v>
       </c>
       <c r="V5">
-        <v>90.67242424763813</v>
+        <v>90.672424247638133</v>
       </c>
       <c r="W5">
         <v>443</v>
@@ -882,7 +981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -932,7 +1031,7 @@
         <v>33</v>
       </c>
       <c r="Q6">
-        <v>2.50490731649467</v>
+        <v>2.5049073164946698</v>
       </c>
       <c r="R6">
         <v>288.3380585556759</v>
@@ -944,7 +1043,7 @@
         <v>12.24242424242424</v>
       </c>
       <c r="U6">
-        <v>2.50490731649467</v>
+        <v>2.5049073164946698</v>
       </c>
       <c r="V6">
         <v>288.3380585556759</v>
@@ -962,7 +1061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1003,7 +1102,7 @@
         <v>0.1</v>
       </c>
       <c r="N7">
-        <v>0.9454545454545454</v>
+        <v>0.94545454545454544</v>
       </c>
       <c r="O7">
         <v>142</v>
@@ -1012,22 +1111,22 @@
         <v>32</v>
       </c>
       <c r="Q7">
-        <v>1.490091154801534</v>
+        <v>1.4900911548015341</v>
       </c>
       <c r="R7">
-        <v>62.31708304635091</v>
+        <v>62.317083046350909</v>
       </c>
       <c r="S7">
         <v>4.4375</v>
       </c>
       <c r="T7">
-        <v>6.777777777777778</v>
+        <v>6.7777777777777777</v>
       </c>
       <c r="U7">
         <v>1.913649286837092</v>
       </c>
       <c r="V7">
-        <v>69.55431283693235</v>
+        <v>69.554312836932354</v>
       </c>
       <c r="W7">
         <v>580</v>
@@ -1042,7 +1141,7 @@
         <v>1.010452961672474</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1095,19 +1194,19 @@
         <v>2.112231364502827</v>
       </c>
       <c r="R8">
-        <v>77.31652953245759</v>
+        <v>77.316529532457594</v>
       </c>
       <c r="S8">
-        <v>8.266666666666667</v>
+        <v>8.2666666666666675</v>
       </c>
       <c r="T8">
-        <v>8.266666666666667</v>
+        <v>8.2666666666666675</v>
       </c>
       <c r="U8">
         <v>2.112231364502827</v>
       </c>
       <c r="V8">
-        <v>77.31652953245759</v>
+        <v>77.316529532457594</v>
       </c>
       <c r="W8">
         <v>292</v>
@@ -1122,7 +1221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1172,10 +1271,10 @@
         <v>13</v>
       </c>
       <c r="Q9">
-        <v>3.431502731157484</v>
+        <v>3.4315027311574839</v>
       </c>
       <c r="R9">
-        <v>344.3904644949527</v>
+        <v>344.39046449495271</v>
       </c>
       <c r="S9">
         <v>30.92307692307692</v>
@@ -1184,10 +1283,10 @@
         <v>30.92307692307692</v>
       </c>
       <c r="U9">
-        <v>3.431502731157484</v>
+        <v>3.4315027311574839</v>
       </c>
       <c r="V9">
-        <v>344.3904644949527</v>
+        <v>344.39046449495271</v>
       </c>
       <c r="W9">
         <v>1174</v>
@@ -1202,7 +1301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1243,7 +1342,7 @@
         <v>0.1</v>
       </c>
       <c r="N10">
-        <v>0.9755351681957186</v>
+        <v>0.97553516819571862</v>
       </c>
       <c r="O10">
         <v>357</v>
@@ -1252,7 +1351,7 @@
         <v>30</v>
       </c>
       <c r="Q10">
-        <v>2.476538400117484</v>
+        <v>2.4765384001174842</v>
       </c>
       <c r="R10">
         <v>252.7038479964755</v>
@@ -1264,10 +1363,10 @@
         <v>25.53846153846154</v>
       </c>
       <c r="U10">
-        <v>3.240185611454952</v>
+        <v>3.2401856114549519</v>
       </c>
       <c r="V10">
-        <v>276.8775870510856</v>
+        <v>276.87758705108558</v>
       </c>
       <c r="W10">
         <v>831</v>
@@ -1279,10 +1378,10 @@
         <v>823</v>
       </c>
       <c r="Z10">
-        <v>1.009720534629405</v>
+        <v>1.0097205346294049</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1323,7 +1422,7 @@
         <v>0.1</v>
       </c>
       <c r="N11">
-        <v>0.8222222222222222</v>
+        <v>0.82222222222222219</v>
       </c>
       <c r="O11">
         <v>77</v>
@@ -1332,10 +1431,10 @@
         <v>32</v>
       </c>
       <c r="Q11">
-        <v>0.8780695190539572</v>
+        <v>0.87806951905395725</v>
       </c>
       <c r="R11">
-        <v>16.90177539027337</v>
+        <v>16.901775390273372</v>
       </c>
       <c r="S11">
         <v>2.40625</v>
@@ -1347,7 +1446,7 @@
         <v>1.547562508716013</v>
       </c>
       <c r="V11">
-        <v>21.52437491283987</v>
+        <v>21.524374912839871</v>
       </c>
       <c r="W11">
         <v>492</v>
@@ -1359,10 +1458,53 @@
         <v>484</v>
       </c>
       <c r="Z11">
-        <v>1.016528925619835</v>
+        <v>1.0165289256198351</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="J12" s="3">
+        <f>AVERAGE(J2:J11)</f>
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="2">
+        <f>AVERAGE(N2:N11)</f>
+        <v>0.97432119358724878</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="2">
+        <f>AVERAGE(Z2:Z11)</f>
+        <v>1.0036702421921713</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="2">
+        <f>MIN(N2:N11)</f>
+        <v>0.82222222222222219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="2">
+        <f>MAX(Z2:Z11)</f>
+        <v>1.0165289256198351</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>